<commit_message>
367 table added to report
</commit_message>
<xml_diff>
--- a/Compsci367/A3/cs367a3/results.xlsx
+++ b/Compsci367/A3/cs367a3/results.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K49"/>
+  <dimension ref="A1:L49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -369,50 +369,55 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>solver</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>problem</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>avg assignments</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>sd assignments</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>avg backtracks</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>sd backtracks</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>avg runtime</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>sd runtime</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>prob sucess</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>avg repair</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>sd repair</t>
         </is>
@@ -422,17 +427,17 @@
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" t="inlineStr">
         <is>
           <t>australia_map</t>
         </is>
       </c>
-      <c r="C2" t="n">
+      <c r="D2" t="n">
         <v>6</v>
       </c>
-      <c r="D2" t="n">
-        <v>0</v>
-      </c>
       <c r="E2" t="n">
         <v>0</v>
       </c>
@@ -440,32 +445,35 @@
         <v>0</v>
       </c>
       <c r="G2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" t="n">
         <v>9.980201721191407e-05</v>
       </c>
-      <c r="H2" t="n">
+      <c r="I2" t="n">
         <v>0.0002994060516357422</v>
       </c>
-      <c r="I2" t="n">
-        <v>100</v>
-      </c>
-      <c r="J2" t="inlineStr"/>
+      <c r="J2" t="n">
+        <v>100</v>
+      </c>
       <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" t="inlineStr">
         <is>
           <t>usa_csp</t>
         </is>
       </c>
-      <c r="C3" t="n">
+      <c r="D3" t="n">
         <v>49</v>
       </c>
-      <c r="D3" t="n">
-        <v>0</v>
-      </c>
       <c r="E3" t="n">
         <v>0</v>
       </c>
@@ -473,230 +481,251 @@
         <v>0</v>
       </c>
       <c r="G3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" t="n">
         <v>0.0007979631423950196</v>
       </c>
-      <c r="H3" t="n">
+      <c r="I3" t="n">
         <v>0.0003989993645743339</v>
       </c>
-      <c r="I3" t="n">
-        <v>100</v>
-      </c>
-      <c r="J3" t="inlineStr"/>
+      <c r="J3" t="n">
+        <v>100</v>
+      </c>
       <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="B4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" t="inlineStr">
         <is>
           <t>zebra</t>
         </is>
       </c>
-      <c r="C4" t="n">
+      <c r="D4" t="n">
         <v>1000</v>
       </c>
-      <c r="D4" t="n">
-        <v>0</v>
-      </c>
       <c r="E4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="n">
         <v>987</v>
       </c>
-      <c r="F4" t="n">
-        <v>0</v>
-      </c>
       <c r="G4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" t="n">
         <v>0.02882020473480225</v>
       </c>
-      <c r="H4" t="n">
+      <c r="I4" t="n">
         <v>0.004683758098977221</v>
       </c>
-      <c r="I4" t="n">
-        <v>0</v>
-      </c>
-      <c r="J4" t="inlineStr"/>
+      <c r="J4" t="n">
+        <v>0</v>
+      </c>
       <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="B5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" t="inlineStr">
         <is>
           <t>10 queens</t>
         </is>
       </c>
-      <c r="C5" t="n">
+      <c r="D5" t="n">
         <v>91</v>
       </c>
-      <c r="D5" t="n">
-        <v>0</v>
-      </c>
       <c r="E5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" t="n">
         <v>81</v>
       </c>
-      <c r="F5" t="n">
-        <v>0</v>
-      </c>
       <c r="G5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" t="n">
         <v>0.001299667358398437</v>
       </c>
-      <c r="H5" t="n">
+      <c r="I5" t="n">
         <v>0.0004641391152584006</v>
       </c>
-      <c r="I5" t="n">
-        <v>100</v>
-      </c>
-      <c r="J5" t="inlineStr"/>
+      <c r="J5" t="n">
+        <v>100</v>
+      </c>
       <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="B6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" t="inlineStr">
         <is>
           <t>30 queens</t>
         </is>
       </c>
-      <c r="C6" t="n">
+      <c r="D6" t="n">
         <v>1000</v>
       </c>
-      <c r="D6" t="n">
-        <v>0</v>
-      </c>
       <c r="E6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" t="n">
         <v>985</v>
       </c>
-      <c r="F6" t="n">
-        <v>0</v>
-      </c>
       <c r="G6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" t="n">
         <v>0.02732822895050049</v>
       </c>
-      <c r="H6" t="n">
+      <c r="I6" t="n">
         <v>0.002202921386052849</v>
       </c>
-      <c r="I6" t="n">
-        <v>0</v>
-      </c>
-      <c r="J6" t="inlineStr"/>
+      <c r="J6" t="n">
+        <v>0</v>
+      </c>
       <c r="K6" t="inlineStr"/>
+      <c r="L6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="B7" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" t="inlineStr">
         <is>
           <t>50 queens</t>
         </is>
       </c>
-      <c r="C7" t="n">
+      <c r="D7" t="n">
         <v>1000</v>
       </c>
-      <c r="D7" t="n">
-        <v>0</v>
-      </c>
       <c r="E7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" t="n">
         <v>966</v>
       </c>
-      <c r="F7" t="n">
-        <v>0</v>
-      </c>
       <c r="G7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" t="n">
         <v>0.05046060085296631</v>
       </c>
-      <c r="H7" t="n">
+      <c r="I7" t="n">
         <v>0.01160625619891778</v>
       </c>
-      <c r="I7" t="n">
-        <v>0</v>
-      </c>
-      <c r="J7" t="inlineStr"/>
+      <c r="J7" t="n">
+        <v>0</v>
+      </c>
       <c r="K7" t="inlineStr"/>
+      <c r="L7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="B8" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" t="inlineStr">
         <is>
           <t>70 queens</t>
         </is>
       </c>
-      <c r="C8" t="n">
+      <c r="D8" t="n">
         <v>1000</v>
       </c>
-      <c r="D8" t="n">
-        <v>0</v>
-      </c>
       <c r="E8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" t="n">
         <v>954</v>
       </c>
-      <c r="F8" t="n">
-        <v>0</v>
-      </c>
       <c r="G8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" t="n">
         <v>0.05854587554931641</v>
       </c>
-      <c r="H8" t="n">
+      <c r="I8" t="n">
         <v>0.006180784769584328</v>
       </c>
-      <c r="I8" t="n">
-        <v>0</v>
-      </c>
-      <c r="J8" t="inlineStr"/>
+      <c r="J8" t="n">
+        <v>0</v>
+      </c>
       <c r="K8" t="inlineStr"/>
+      <c r="L8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="B9" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" t="inlineStr">
         <is>
           <t>90 queens</t>
         </is>
       </c>
-      <c r="C9" t="n">
+      <c r="D9" t="n">
         <v>1000</v>
       </c>
-      <c r="D9" t="n">
-        <v>0</v>
-      </c>
       <c r="E9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" t="n">
         <v>941</v>
       </c>
-      <c r="F9" t="n">
-        <v>0</v>
-      </c>
       <c r="G9" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" t="n">
         <v>0.07141082286834717</v>
       </c>
-      <c r="H9" t="n">
+      <c r="I9" t="n">
         <v>0.002375000806616545</v>
       </c>
-      <c r="I9" t="n">
-        <v>0</v>
-      </c>
-      <c r="J9" t="inlineStr"/>
+      <c r="J9" t="n">
+        <v>0</v>
+      </c>
       <c r="K9" t="inlineStr"/>
+      <c r="L9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B10" t="inlineStr">
+      <c r="B10" t="n">
+        <v>2</v>
+      </c>
+      <c r="C10" t="inlineStr">
         <is>
           <t>australia_map</t>
         </is>
       </c>
-      <c r="C10" t="n">
+      <c r="D10" t="n">
         <v>6</v>
       </c>
-      <c r="D10" t="n">
-        <v>0</v>
-      </c>
       <c r="E10" t="n">
         <v>0</v>
       </c>
@@ -710,26 +739,29 @@
         <v>0</v>
       </c>
       <c r="I10" t="n">
-        <v>100</v>
-      </c>
-      <c r="J10" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="J10" t="n">
+        <v>100</v>
+      </c>
       <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="B11" t="inlineStr">
+      <c r="B11" t="n">
+        <v>2</v>
+      </c>
+      <c r="C11" t="inlineStr">
         <is>
           <t>usa_csp</t>
         </is>
       </c>
-      <c r="C11" t="n">
+      <c r="D11" t="n">
         <v>49</v>
       </c>
-      <c r="D11" t="n">
-        <v>0</v>
-      </c>
       <c r="E11" t="n">
         <v>0</v>
       </c>
@@ -737,230 +769,251 @@
         <v>0</v>
       </c>
       <c r="G11" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" t="n">
         <v>0.0006967544555664063</v>
       </c>
-      <c r="H11" t="n">
+      <c r="I11" t="n">
         <v>0.0004561516471535193</v>
       </c>
-      <c r="I11" t="n">
-        <v>100</v>
-      </c>
-      <c r="J11" t="inlineStr"/>
+      <c r="J11" t="n">
+        <v>100</v>
+      </c>
       <c r="K11" t="inlineStr"/>
+      <c r="L11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="B12" t="inlineStr">
+      <c r="B12" t="n">
+        <v>2</v>
+      </c>
+      <c r="C12" t="inlineStr">
         <is>
           <t>zebra</t>
         </is>
       </c>
-      <c r="C12" t="n">
+      <c r="D12" t="n">
         <v>1000</v>
       </c>
-      <c r="D12" t="n">
-        <v>0</v>
-      </c>
       <c r="E12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" t="n">
         <v>650</v>
       </c>
-      <c r="F12" t="n">
-        <v>0</v>
-      </c>
       <c r="G12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H12" t="n">
         <v>0.02153792381286621</v>
       </c>
-      <c r="H12" t="n">
+      <c r="I12" t="n">
         <v>0.004338887604501171</v>
       </c>
-      <c r="I12" t="n">
-        <v>0</v>
-      </c>
-      <c r="J12" t="inlineStr"/>
+      <c r="J12" t="n">
+        <v>0</v>
+      </c>
       <c r="K12" t="inlineStr"/>
+      <c r="L12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="B13" t="inlineStr">
+      <c r="B13" t="n">
+        <v>2</v>
+      </c>
+      <c r="C13" t="inlineStr">
         <is>
           <t>10 queens</t>
         </is>
       </c>
-      <c r="C13" t="n">
+      <c r="D13" t="n">
         <v>73</v>
       </c>
-      <c r="D13" t="n">
-        <v>0</v>
-      </c>
       <c r="E13" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" t="n">
         <v>35</v>
       </c>
-      <c r="F13" t="n">
-        <v>0</v>
-      </c>
       <c r="G13" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" t="n">
         <v>0.001099634170532227</v>
       </c>
-      <c r="H13" t="n">
+      <c r="I13" t="n">
         <v>0.0005436191197662754</v>
       </c>
-      <c r="I13" t="n">
-        <v>100</v>
-      </c>
-      <c r="J13" t="inlineStr"/>
+      <c r="J13" t="n">
+        <v>100</v>
+      </c>
       <c r="K13" t="inlineStr"/>
+      <c r="L13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="B14" t="inlineStr">
+      <c r="B14" t="n">
+        <v>2</v>
+      </c>
+      <c r="C14" t="inlineStr">
         <is>
           <t>30 queens</t>
         </is>
       </c>
-      <c r="C14" t="n">
+      <c r="D14" t="n">
         <v>1000</v>
       </c>
-      <c r="D14" t="n">
-        <v>0</v>
-      </c>
       <c r="E14" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" t="n">
         <v>570</v>
       </c>
-      <c r="F14" t="n">
-        <v>0</v>
-      </c>
       <c r="G14" t="n">
+        <v>0</v>
+      </c>
+      <c r="H14" t="n">
         <v>0.02363748550415039</v>
       </c>
-      <c r="H14" t="n">
+      <c r="I14" t="n">
         <v>0.001276176172476934</v>
       </c>
-      <c r="I14" t="n">
-        <v>0</v>
-      </c>
-      <c r="J14" t="inlineStr"/>
+      <c r="J14" t="n">
+        <v>0</v>
+      </c>
       <c r="K14" t="inlineStr"/>
+      <c r="L14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="B15" t="inlineStr">
+      <c r="B15" t="n">
+        <v>2</v>
+      </c>
+      <c r="C15" t="inlineStr">
         <is>
           <t>50 queens</t>
         </is>
       </c>
-      <c r="C15" t="n">
+      <c r="D15" t="n">
         <v>1000</v>
       </c>
-      <c r="D15" t="n">
-        <v>0</v>
-      </c>
       <c r="E15" t="n">
+        <v>0</v>
+      </c>
+      <c r="F15" t="n">
         <v>568</v>
       </c>
-      <c r="F15" t="n">
-        <v>0</v>
-      </c>
       <c r="G15" t="n">
+        <v>0</v>
+      </c>
+      <c r="H15" t="n">
         <v>0.04547560214996338</v>
       </c>
-      <c r="H15" t="n">
+      <c r="I15" t="n">
         <v>0.001362392235760131</v>
       </c>
-      <c r="I15" t="n">
-        <v>0</v>
-      </c>
-      <c r="J15" t="inlineStr"/>
+      <c r="J15" t="n">
+        <v>0</v>
+      </c>
       <c r="K15" t="inlineStr"/>
+      <c r="L15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="B16" t="inlineStr">
+      <c r="B16" t="n">
+        <v>2</v>
+      </c>
+      <c r="C16" t="inlineStr">
         <is>
           <t>70 queens</t>
         </is>
       </c>
-      <c r="C16" t="n">
+      <c r="D16" t="n">
         <v>1000</v>
       </c>
-      <c r="D16" t="n">
-        <v>0</v>
-      </c>
       <c r="E16" t="n">
+        <v>0</v>
+      </c>
+      <c r="F16" t="n">
         <v>542</v>
       </c>
-      <c r="F16" t="n">
-        <v>0</v>
-      </c>
       <c r="G16" t="n">
+        <v>0</v>
+      </c>
+      <c r="H16" t="n">
         <v>0.07749276161193848</v>
       </c>
-      <c r="H16" t="n">
+      <c r="I16" t="n">
         <v>0.002441514138542442</v>
       </c>
-      <c r="I16" t="n">
-        <v>0</v>
-      </c>
-      <c r="J16" t="inlineStr"/>
+      <c r="J16" t="n">
+        <v>0</v>
+      </c>
       <c r="K16" t="inlineStr"/>
+      <c r="L16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="B17" t="inlineStr">
+      <c r="B17" t="n">
+        <v>2</v>
+      </c>
+      <c r="C17" t="inlineStr">
         <is>
           <t>90 queens</t>
         </is>
       </c>
-      <c r="C17" t="n">
+      <c r="D17" t="n">
         <v>1000</v>
       </c>
-      <c r="D17" t="n">
-        <v>0</v>
-      </c>
       <c r="E17" t="n">
+        <v>0</v>
+      </c>
+      <c r="F17" t="n">
         <v>538</v>
       </c>
-      <c r="F17" t="n">
-        <v>0</v>
-      </c>
       <c r="G17" t="n">
+        <v>0</v>
+      </c>
+      <c r="H17" t="n">
         <v>0.1520934581756592</v>
       </c>
-      <c r="H17" t="n">
+      <c r="I17" t="n">
         <v>0.03798458949332571</v>
       </c>
-      <c r="I17" t="n">
-        <v>0</v>
-      </c>
-      <c r="J17" t="inlineStr"/>
+      <c r="J17" t="n">
+        <v>0</v>
+      </c>
       <c r="K17" t="inlineStr"/>
+      <c r="L17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="B18" t="inlineStr">
+      <c r="B18" t="n">
+        <v>3</v>
+      </c>
+      <c r="C18" t="inlineStr">
         <is>
           <t>australia_map</t>
         </is>
       </c>
-      <c r="C18" t="n">
+      <c r="D18" t="n">
         <v>6</v>
       </c>
-      <c r="D18" t="n">
-        <v>0</v>
-      </c>
       <c r="E18" t="n">
         <v>0</v>
       </c>
@@ -968,32 +1021,35 @@
         <v>0</v>
       </c>
       <c r="G18" t="n">
+        <v>0</v>
+      </c>
+      <c r="H18" t="n">
         <v>0.0002989292144775391</v>
       </c>
-      <c r="H18" t="n">
+      <c r="I18" t="n">
         <v>0.000456622432137646</v>
       </c>
-      <c r="I18" t="n">
-        <v>100</v>
-      </c>
-      <c r="J18" t="inlineStr"/>
+      <c r="J18" t="n">
+        <v>100</v>
+      </c>
       <c r="K18" t="inlineStr"/>
+      <c r="L18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
         <v>17</v>
       </c>
-      <c r="B19" t="inlineStr">
+      <c r="B19" t="n">
+        <v>3</v>
+      </c>
+      <c r="C19" t="inlineStr">
         <is>
           <t>usa_csp</t>
         </is>
       </c>
-      <c r="C19" t="n">
+      <c r="D19" t="n">
         <v>49</v>
       </c>
-      <c r="D19" t="n">
-        <v>0</v>
-      </c>
       <c r="E19" t="n">
         <v>0</v>
       </c>
@@ -1001,494 +1057,539 @@
         <v>0</v>
       </c>
       <c r="G19" t="n">
+        <v>0</v>
+      </c>
+      <c r="H19" t="n">
         <v>0.00359036922454834</v>
       </c>
-      <c r="H19" t="n">
+      <c r="I19" t="n">
         <v>0.0004895617048299769</v>
       </c>
-      <c r="I19" t="n">
-        <v>100</v>
-      </c>
-      <c r="J19" t="inlineStr"/>
+      <c r="J19" t="n">
+        <v>100</v>
+      </c>
       <c r="K19" t="inlineStr"/>
+      <c r="L19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="B20" t="inlineStr">
+      <c r="B20" t="n">
+        <v>3</v>
+      </c>
+      <c r="C20" t="inlineStr">
         <is>
           <t>zebra</t>
         </is>
       </c>
-      <c r="C20" t="n">
+      <c r="D20" t="n">
         <v>1000</v>
       </c>
-      <c r="D20" t="n">
-        <v>0</v>
-      </c>
       <c r="E20" t="n">
+        <v>0</v>
+      </c>
+      <c r="F20" t="n">
         <v>989</v>
       </c>
-      <c r="F20" t="n">
-        <v>0</v>
-      </c>
       <c r="G20" t="n">
+        <v>0</v>
+      </c>
+      <c r="H20" t="n">
         <v>0.09863381385803223</v>
       </c>
-      <c r="H20" t="n">
+      <c r="I20" t="n">
         <v>0.016306411812419</v>
       </c>
-      <c r="I20" t="n">
-        <v>0</v>
-      </c>
-      <c r="J20" t="inlineStr"/>
+      <c r="J20" t="n">
+        <v>0</v>
+      </c>
       <c r="K20" t="inlineStr"/>
+      <c r="L20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
         <v>19</v>
       </c>
-      <c r="B21" t="inlineStr">
+      <c r="B21" t="n">
+        <v>3</v>
+      </c>
+      <c r="C21" t="inlineStr">
         <is>
           <t>10 queens</t>
         </is>
       </c>
-      <c r="C21" t="n">
+      <c r="D21" t="n">
         <v>50</v>
       </c>
-      <c r="D21" t="n">
-        <v>0</v>
-      </c>
       <c r="E21" t="n">
+        <v>0</v>
+      </c>
+      <c r="F21" t="n">
         <v>40</v>
       </c>
-      <c r="F21" t="n">
-        <v>0</v>
-      </c>
       <c r="G21" t="n">
+        <v>0</v>
+      </c>
+      <c r="H21" t="n">
         <v>0.008081436157226562</v>
       </c>
-      <c r="H21" t="n">
+      <c r="I21" t="n">
         <v>0.0007063453945446101</v>
       </c>
-      <c r="I21" t="n">
-        <v>100</v>
-      </c>
-      <c r="J21" t="inlineStr"/>
+      <c r="J21" t="n">
+        <v>100</v>
+      </c>
       <c r="K21" t="inlineStr"/>
+      <c r="L21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="B22" t="inlineStr">
+      <c r="B22" t="n">
+        <v>3</v>
+      </c>
+      <c r="C22" t="inlineStr">
         <is>
           <t>30 queens</t>
         </is>
       </c>
-      <c r="C22" t="n">
+      <c r="D22" t="n">
         <v>1000</v>
       </c>
-      <c r="D22" t="n">
-        <v>0</v>
-      </c>
       <c r="E22" t="n">
+        <v>0</v>
+      </c>
+      <c r="F22" t="n">
         <v>979</v>
       </c>
-      <c r="F22" t="n">
-        <v>0</v>
-      </c>
       <c r="G22" t="n">
+        <v>0</v>
+      </c>
+      <c r="H22" t="n">
         <v>0.8031146764755249</v>
       </c>
-      <c r="H22" t="n">
+      <c r="I22" t="n">
         <v>0.1328208255567625</v>
       </c>
-      <c r="I22" t="n">
-        <v>0</v>
-      </c>
-      <c r="J22" t="inlineStr"/>
+      <c r="J22" t="n">
+        <v>0</v>
+      </c>
       <c r="K22" t="inlineStr"/>
+      <c r="L22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
         <v>21</v>
       </c>
-      <c r="B23" t="inlineStr">
+      <c r="B23" t="n">
+        <v>3</v>
+      </c>
+      <c r="C23" t="inlineStr">
         <is>
           <t>50 queens</t>
         </is>
       </c>
-      <c r="C23" t="n">
+      <c r="D23" t="n">
         <v>1000</v>
       </c>
-      <c r="D23" t="n">
-        <v>0</v>
-      </c>
       <c r="E23" t="n">
+        <v>0</v>
+      </c>
+      <c r="F23" t="n">
         <v>966</v>
       </c>
-      <c r="F23" t="n">
-        <v>0</v>
-      </c>
       <c r="G23" t="n">
+        <v>0</v>
+      </c>
+      <c r="H23" t="n">
         <v>2.515515971183777</v>
       </c>
-      <c r="H23" t="n">
+      <c r="I23" t="n">
         <v>0.2687823204330491</v>
       </c>
-      <c r="I23" t="n">
-        <v>0</v>
-      </c>
-      <c r="J23" t="inlineStr"/>
+      <c r="J23" t="n">
+        <v>0</v>
+      </c>
       <c r="K23" t="inlineStr"/>
+      <c r="L23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="B24" t="inlineStr">
+      <c r="B24" t="n">
+        <v>3</v>
+      </c>
+      <c r="C24" t="inlineStr">
         <is>
           <t>70 queens</t>
         </is>
       </c>
-      <c r="C24" t="n">
+      <c r="D24" t="n">
         <v>1000</v>
       </c>
-      <c r="D24" t="n">
-        <v>0</v>
-      </c>
       <c r="E24" t="n">
+        <v>0</v>
+      </c>
+      <c r="F24" t="n">
         <v>953</v>
       </c>
-      <c r="F24" t="n">
-        <v>0</v>
-      </c>
       <c r="G24" t="n">
+        <v>0</v>
+      </c>
+      <c r="H24" t="n">
         <v>5.77183883190155</v>
       </c>
-      <c r="H24" t="n">
+      <c r="I24" t="n">
         <v>0.6803534368776827</v>
       </c>
-      <c r="I24" t="n">
-        <v>0</v>
-      </c>
-      <c r="J24" t="inlineStr"/>
+      <c r="J24" t="n">
+        <v>0</v>
+      </c>
       <c r="K24" t="inlineStr"/>
+      <c r="L24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
         <v>23</v>
       </c>
-      <c r="B25" t="inlineStr">
+      <c r="B25" t="n">
+        <v>3</v>
+      </c>
+      <c r="C25" t="inlineStr">
         <is>
           <t>90 queens</t>
         </is>
       </c>
-      <c r="C25" t="n">
+      <c r="D25" t="n">
         <v>1000</v>
       </c>
-      <c r="D25" t="n">
-        <v>0</v>
-      </c>
       <c r="E25" t="n">
+        <v>0</v>
+      </c>
+      <c r="F25" t="n">
         <v>942</v>
       </c>
-      <c r="F25" t="n">
-        <v>0</v>
-      </c>
       <c r="G25" t="n">
+        <v>0</v>
+      </c>
+      <c r="H25" t="n">
         <v>12.93859448432922</v>
       </c>
-      <c r="H25" t="n">
+      <c r="I25" t="n">
         <v>0.8248415034101568</v>
       </c>
-      <c r="I25" t="n">
-        <v>0</v>
-      </c>
-      <c r="J25" t="inlineStr"/>
+      <c r="J25" t="n">
+        <v>0</v>
+      </c>
       <c r="K25" t="inlineStr"/>
+      <c r="L25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
         <v>24</v>
       </c>
-      <c r="B26" t="inlineStr">
+      <c r="B26" t="n">
+        <v>4</v>
+      </c>
+      <c r="C26" t="inlineStr">
         <is>
           <t>australia_map</t>
         </is>
       </c>
-      <c r="C26" t="n">
+      <c r="D26" t="n">
         <v>9.199999999999999</v>
       </c>
-      <c r="D26" t="n">
+      <c r="E26" t="n">
         <v>5.230678732248808</v>
       </c>
-      <c r="E26" t="n">
+      <c r="F26" t="n">
         <v>3.2</v>
       </c>
-      <c r="F26" t="n">
+      <c r="G26" t="n">
         <v>5.230678732248808</v>
       </c>
-      <c r="G26" t="n">
+      <c r="H26" t="n">
         <v>0.000199437141418457</v>
       </c>
-      <c r="H26" t="n">
+      <c r="I26" t="n">
         <v>0.0003988742863996543</v>
       </c>
-      <c r="I26" t="n">
-        <v>100</v>
-      </c>
-      <c r="J26" t="inlineStr"/>
+      <c r="J26" t="n">
+        <v>100</v>
+      </c>
       <c r="K26" t="inlineStr"/>
+      <c r="L26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="B27" t="inlineStr">
+      <c r="B27" t="n">
+        <v>4</v>
+      </c>
+      <c r="C27" t="inlineStr">
         <is>
           <t>usa_csp</t>
         </is>
       </c>
-      <c r="C27" t="n">
+      <c r="D27" t="n">
         <v>904.9</v>
       </c>
-      <c r="D27" t="n">
+      <c r="E27" t="n">
         <v>285.3</v>
       </c>
-      <c r="E27" t="n">
+      <c r="F27" t="n">
         <v>863.1</v>
       </c>
-      <c r="F27" t="n">
+      <c r="G27" t="n">
         <v>287.7163359978018</v>
       </c>
-      <c r="G27" t="n">
+      <c r="H27" t="n">
         <v>0.03560478687286377</v>
       </c>
-      <c r="H27" t="n">
+      <c r="I27" t="n">
         <v>0.012304755594113</v>
       </c>
-      <c r="I27" t="n">
+      <c r="J27" t="n">
         <v>10</v>
       </c>
-      <c r="J27" t="inlineStr"/>
       <c r="K27" t="inlineStr"/>
+      <c r="L27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
         <v>26</v>
       </c>
-      <c r="B28" t="inlineStr">
+      <c r="B28" t="n">
+        <v>4</v>
+      </c>
+      <c r="C28" t="inlineStr">
         <is>
           <t>zebra</t>
         </is>
       </c>
-      <c r="C28" t="n">
+      <c r="D28" t="n">
         <v>1000</v>
       </c>
-      <c r="D28" t="n">
-        <v>0</v>
-      </c>
       <c r="E28" t="n">
+        <v>0</v>
+      </c>
+      <c r="F28" t="n">
         <v>986.9</v>
       </c>
-      <c r="F28" t="n">
+      <c r="G28" t="n">
         <v>2.736786436680802</v>
       </c>
-      <c r="G28" t="n">
+      <c r="H28" t="n">
         <v>0.08010003566741944</v>
       </c>
-      <c r="H28" t="n">
+      <c r="I28" t="n">
         <v>0.005094757787493845</v>
       </c>
-      <c r="I28" t="n">
-        <v>0</v>
-      </c>
-      <c r="J28" t="inlineStr"/>
+      <c r="J28" t="n">
+        <v>0</v>
+      </c>
       <c r="K28" t="inlineStr"/>
+      <c r="L28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
         <v>27</v>
       </c>
-      <c r="B29" t="inlineStr">
+      <c r="B29" t="n">
+        <v>4</v>
+      </c>
+      <c r="C29" t="inlineStr">
         <is>
           <t>10 queens</t>
         </is>
       </c>
-      <c r="C29" t="n">
+      <c r="D29" t="n">
         <v>224.6</v>
       </c>
-      <c r="D29" t="n">
+      <c r="E29" t="n">
         <v>278.8469831287403</v>
       </c>
-      <c r="E29" t="n">
+      <c r="F29" t="n">
         <v>214.6</v>
       </c>
-      <c r="F29" t="n">
+      <c r="G29" t="n">
         <v>278.8469831287403</v>
       </c>
-      <c r="G29" t="n">
+      <c r="H29" t="n">
         <v>0.005083847045898438</v>
       </c>
-      <c r="H29" t="n">
+      <c r="I29" t="n">
         <v>0.006497210120874403</v>
       </c>
-      <c r="I29" t="n">
-        <v>100</v>
-      </c>
-      <c r="J29" t="inlineStr"/>
+      <c r="J29" t="n">
+        <v>100</v>
+      </c>
       <c r="K29" t="inlineStr"/>
+      <c r="L29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
         <v>28</v>
       </c>
-      <c r="B30" t="inlineStr">
+      <c r="B30" t="n">
+        <v>4</v>
+      </c>
+      <c r="C30" t="inlineStr">
         <is>
           <t>30 queens</t>
         </is>
       </c>
-      <c r="C30" t="n">
+      <c r="D30" t="n">
         <v>818.1</v>
       </c>
-      <c r="D30" t="n">
+      <c r="E30" t="n">
         <v>248.8619898658692</v>
       </c>
-      <c r="E30" t="n">
+      <c r="F30" t="n">
         <v>790.3</v>
       </c>
-      <c r="F30" t="n">
+      <c r="G30" t="n">
         <v>250.4723737261258</v>
       </c>
-      <c r="G30" t="n">
+      <c r="H30" t="n">
         <v>0.04328675270080566</v>
       </c>
-      <c r="H30" t="n">
+      <c r="I30" t="n">
         <v>0.01413425565778744</v>
       </c>
-      <c r="I30" t="n">
+      <c r="J30" t="n">
         <v>40</v>
       </c>
-      <c r="J30" t="inlineStr"/>
       <c r="K30" t="inlineStr"/>
+      <c r="L30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
         <v>29</v>
       </c>
-      <c r="B31" t="inlineStr">
+      <c r="B31" t="n">
+        <v>4</v>
+      </c>
+      <c r="C31" t="inlineStr">
         <is>
           <t>50 queens</t>
         </is>
       </c>
-      <c r="C31" t="n">
+      <c r="D31" t="n">
         <v>771.8</v>
       </c>
-      <c r="D31" t="n">
+      <c r="E31" t="n">
         <v>351.1520468401117</v>
       </c>
-      <c r="E31" t="n">
+      <c r="F31" t="n">
         <v>725.3</v>
       </c>
-      <c r="F31" t="n">
+      <c r="G31" t="n">
         <v>353.4337420224617</v>
       </c>
-      <c r="G31" t="n">
+      <c r="H31" t="n">
         <v>0.06164109706878662</v>
       </c>
-      <c r="H31" t="n">
+      <c r="I31" t="n">
         <v>0.02816250735564435</v>
       </c>
-      <c r="I31" t="n">
+      <c r="J31" t="n">
         <v>40</v>
       </c>
-      <c r="J31" t="inlineStr"/>
       <c r="K31" t="inlineStr"/>
+      <c r="L31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="B32" t="inlineStr">
+      <c r="B32" t="n">
+        <v>4</v>
+      </c>
+      <c r="C32" t="inlineStr">
         <is>
           <t>70 queens</t>
         </is>
       </c>
-      <c r="C32" t="n">
+      <c r="D32" t="n">
         <v>907.8</v>
       </c>
-      <c r="D32" t="n">
+      <c r="E32" t="n">
         <v>167.7526750904438</v>
       </c>
-      <c r="E32" t="n">
+      <c r="F32" t="n">
         <v>842.2</v>
       </c>
-      <c r="F32" t="n">
+      <c r="G32" t="n">
         <v>170.1974147864767</v>
       </c>
-      <c r="G32" t="n">
+      <c r="H32" t="n">
         <v>0.1402248620986938</v>
       </c>
-      <c r="H32" t="n">
+      <c r="I32" t="n">
         <v>0.03586647067242593</v>
       </c>
-      <c r="I32" t="n">
+      <c r="J32" t="n">
         <v>40</v>
       </c>
-      <c r="J32" t="inlineStr"/>
       <c r="K32" t="inlineStr"/>
+      <c r="L32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
         <v>31</v>
       </c>
-      <c r="B33" t="inlineStr">
+      <c r="B33" t="n">
+        <v>4</v>
+      </c>
+      <c r="C33" t="inlineStr">
         <is>
           <t>90 queens</t>
         </is>
       </c>
-      <c r="C33" t="n">
+      <c r="D33" t="n">
         <v>1000</v>
       </c>
-      <c r="D33" t="n">
-        <v>0</v>
-      </c>
       <c r="E33" t="n">
+        <v>0</v>
+      </c>
+      <c r="F33" t="n">
         <v>919</v>
       </c>
-      <c r="F33" t="n">
+      <c r="G33" t="n">
         <v>2.645751311064591</v>
       </c>
-      <c r="G33" t="n">
+      <c r="H33" t="n">
         <v>0.1363384962081909</v>
       </c>
-      <c r="H33" t="n">
+      <c r="I33" t="n">
         <v>0.004461711319863212</v>
       </c>
-      <c r="I33" t="n">
-        <v>0</v>
-      </c>
-      <c r="J33" t="inlineStr"/>
+      <c r="J33" t="n">
+        <v>0</v>
+      </c>
       <c r="K33" t="inlineStr"/>
+      <c r="L33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
         <v>32</v>
       </c>
-      <c r="B34" t="inlineStr">
+      <c r="B34" t="n">
+        <v>5</v>
+      </c>
+      <c r="C34" t="inlineStr">
         <is>
           <t>australia_map</t>
         </is>
       </c>
-      <c r="C34" t="n">
+      <c r="D34" t="n">
         <v>6</v>
       </c>
-      <c r="D34" t="n">
-        <v>0</v>
-      </c>
       <c r="E34" t="n">
         <v>0</v>
       </c>
@@ -1496,32 +1597,35 @@
         <v>0</v>
       </c>
       <c r="G34" t="n">
+        <v>0</v>
+      </c>
+      <c r="H34" t="n">
         <v>0.0003988981246948242</v>
       </c>
-      <c r="H34" t="n">
+      <c r="I34" t="n">
         <v>0.0004885485415073733</v>
       </c>
-      <c r="I34" t="n">
-        <v>100</v>
-      </c>
-      <c r="J34" t="inlineStr"/>
+      <c r="J34" t="n">
+        <v>100</v>
+      </c>
       <c r="K34" t="inlineStr"/>
+      <c r="L34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
         <v>33</v>
       </c>
-      <c r="B35" t="inlineStr">
+      <c r="B35" t="n">
+        <v>5</v>
+      </c>
+      <c r="C35" t="inlineStr">
         <is>
           <t>usa_csp</t>
         </is>
       </c>
-      <c r="C35" t="n">
+      <c r="D35" t="n">
         <v>49</v>
       </c>
-      <c r="D35" t="n">
-        <v>0</v>
-      </c>
       <c r="E35" t="n">
         <v>0</v>
       </c>
@@ -1529,245 +1633,269 @@
         <v>0</v>
       </c>
       <c r="G35" t="n">
+        <v>0</v>
+      </c>
+      <c r="H35" t="n">
         <v>0.005288004875183105</v>
       </c>
-      <c r="H35" t="n">
+      <c r="I35" t="n">
         <v>0.0004598761933869416</v>
       </c>
-      <c r="I35" t="n">
-        <v>100</v>
-      </c>
-      <c r="J35" t="inlineStr"/>
+      <c r="J35" t="n">
+        <v>100</v>
+      </c>
       <c r="K35" t="inlineStr"/>
+      <c r="L35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
         <v>34</v>
       </c>
-      <c r="B36" t="inlineStr">
+      <c r="B36" t="n">
+        <v>5</v>
+      </c>
+      <c r="C36" t="inlineStr">
         <is>
           <t>zebra</t>
         </is>
       </c>
-      <c r="C36" t="n">
+      <c r="D36" t="n">
         <v>45.5</v>
       </c>
-      <c r="D36" t="n">
+      <c r="E36" t="n">
         <v>2.974894956128703</v>
       </c>
-      <c r="E36" t="n">
+      <c r="F36" t="n">
         <v>20.5</v>
       </c>
-      <c r="F36" t="n">
+      <c r="G36" t="n">
         <v>2.974894956128703</v>
       </c>
-      <c r="G36" t="n">
+      <c r="H36" t="n">
         <v>0.007677292823791504</v>
       </c>
-      <c r="H36" t="n">
+      <c r="I36" t="n">
         <v>0.000455999818790893</v>
       </c>
-      <c r="I36" t="n">
-        <v>100</v>
-      </c>
-      <c r="J36" t="inlineStr"/>
+      <c r="J36" t="n">
+        <v>100</v>
+      </c>
       <c r="K36" t="inlineStr"/>
+      <c r="L36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
         <v>35</v>
       </c>
-      <c r="B37" t="inlineStr">
+      <c r="B37" t="n">
+        <v>5</v>
+      </c>
+      <c r="C37" t="inlineStr">
         <is>
           <t>10 queens</t>
         </is>
       </c>
-      <c r="C37" t="n">
+      <c r="D37" t="n">
         <v>18.1</v>
       </c>
-      <c r="D37" t="n">
+      <c r="E37" t="n">
         <v>7.286288492778747</v>
       </c>
-      <c r="E37" t="n">
+      <c r="F37" t="n">
         <v>8.1</v>
       </c>
-      <c r="F37" t="n">
+      <c r="G37" t="n">
         <v>7.286288492778747</v>
       </c>
-      <c r="G37" t="n">
+      <c r="H37" t="n">
         <v>0.004787254333496094</v>
       </c>
-      <c r="H37" t="n">
+      <c r="I37" t="n">
         <v>0.002082784306480197</v>
       </c>
-      <c r="I37" t="n">
-        <v>100</v>
-      </c>
-      <c r="J37" t="inlineStr"/>
+      <c r="J37" t="n">
+        <v>100</v>
+      </c>
       <c r="K37" t="inlineStr"/>
+      <c r="L37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
         <v>36</v>
       </c>
-      <c r="B38" t="inlineStr">
+      <c r="B38" t="n">
+        <v>5</v>
+      </c>
+      <c r="C38" t="inlineStr">
         <is>
           <t>30 queens</t>
         </is>
       </c>
-      <c r="C38" t="n">
+      <c r="D38" t="n">
         <v>49.8</v>
       </c>
-      <c r="D38" t="n">
+      <c r="E38" t="n">
         <v>28.3365488371467</v>
       </c>
-      <c r="E38" t="n">
+      <c r="F38" t="n">
         <v>19.8</v>
       </c>
-      <c r="F38" t="n">
+      <c r="G38" t="n">
         <v>28.3365488371467</v>
       </c>
-      <c r="G38" t="n">
+      <c r="H38" t="n">
         <v>0.1319009304046631</v>
       </c>
-      <c r="H38" t="n">
+      <c r="I38" t="n">
         <v>0.02832498865796318</v>
       </c>
-      <c r="I38" t="n">
-        <v>100</v>
-      </c>
-      <c r="J38" t="inlineStr"/>
+      <c r="J38" t="n">
+        <v>100</v>
+      </c>
       <c r="K38" t="inlineStr"/>
+      <c r="L38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
         <v>37</v>
       </c>
-      <c r="B39" t="inlineStr">
+      <c r="B39" t="n">
+        <v>5</v>
+      </c>
+      <c r="C39" t="inlineStr">
         <is>
           <t>50 queens</t>
         </is>
       </c>
-      <c r="C39" t="n">
+      <c r="D39" t="n">
         <v>82</v>
       </c>
-      <c r="D39" t="n">
+      <c r="E39" t="n">
         <v>41.5547831181923</v>
       </c>
-      <c r="E39" t="n">
+      <c r="F39" t="n">
         <v>32</v>
       </c>
-      <c r="F39" t="n">
+      <c r="G39" t="n">
         <v>41.5547831181923</v>
       </c>
-      <c r="G39" t="n">
+      <c r="H39" t="n">
         <v>1.162538599967956</v>
       </c>
-      <c r="H39" t="n">
+      <c r="I39" t="n">
         <v>0.3519248061987034</v>
       </c>
-      <c r="I39" t="n">
-        <v>100</v>
-      </c>
-      <c r="J39" t="inlineStr"/>
+      <c r="J39" t="n">
+        <v>100</v>
+      </c>
       <c r="K39" t="inlineStr"/>
+      <c r="L39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
         <v>38</v>
       </c>
-      <c r="B40" t="inlineStr">
+      <c r="B40" t="n">
+        <v>5</v>
+      </c>
+      <c r="C40" t="inlineStr">
         <is>
           <t>70 queens</t>
         </is>
       </c>
-      <c r="C40" t="n">
+      <c r="D40" t="n">
         <v>446.5</v>
       </c>
-      <c r="D40" t="n">
+      <c r="E40" t="n">
         <v>390.8834225187863</v>
       </c>
-      <c r="E40" t="n">
+      <c r="F40" t="n">
         <v>380.6</v>
       </c>
-      <c r="F40" t="n">
+      <c r="G40" t="n">
         <v>396.6991807402682</v>
       </c>
-      <c r="G40" t="n">
+      <c r="H40" t="n">
         <v>4.049901533126831</v>
       </c>
-      <c r="H40" t="n">
+      <c r="I40" t="n">
         <v>1.113617423103301</v>
       </c>
-      <c r="I40" t="n">
+      <c r="J40" t="n">
         <v>70</v>
       </c>
-      <c r="J40" t="inlineStr"/>
       <c r="K40" t="inlineStr"/>
+      <c r="L40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
         <v>39</v>
       </c>
-      <c r="B41" t="inlineStr">
+      <c r="B41" t="n">
+        <v>5</v>
+      </c>
+      <c r="C41" t="inlineStr">
         <is>
           <t>90 queens</t>
         </is>
       </c>
-      <c r="C41" t="n">
+      <c r="D41" t="n">
         <v>356.2</v>
       </c>
-      <c r="D41" t="n">
+      <c r="E41" t="n">
         <v>320.1361585325844</v>
       </c>
-      <c r="E41" t="n">
+      <c r="F41" t="n">
         <v>267.5</v>
       </c>
-      <c r="F41" t="n">
+      <c r="G41" t="n">
         <v>322.7634582786595</v>
       </c>
-      <c r="G41" t="n">
+      <c r="H41" t="n">
         <v>10.12057273387909</v>
       </c>
-      <c r="H41" t="n">
+      <c r="I41" t="n">
         <v>1.770101783839181</v>
       </c>
-      <c r="I41" t="n">
+      <c r="J41" t="n">
         <v>90</v>
       </c>
-      <c r="J41" t="inlineStr"/>
       <c r="K41" t="inlineStr"/>
+      <c r="L41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
         <v>40</v>
       </c>
-      <c r="B42" t="inlineStr">
+      <c r="B42" t="n">
+        <v>6</v>
+      </c>
+      <c r="C42" t="inlineStr">
         <is>
           <t>australia_map</t>
         </is>
       </c>
-      <c r="C42" t="n">
+      <c r="D42" t="n">
         <v>6</v>
       </c>
-      <c r="D42" t="n">
-        <v>0</v>
-      </c>
-      <c r="E42" t="inlineStr"/>
+      <c r="E42" t="n">
+        <v>0</v>
+      </c>
       <c r="F42" t="inlineStr"/>
-      <c r="G42" t="n">
+      <c r="G42" t="inlineStr"/>
+      <c r="H42" t="n">
         <v>9.97304916381836e-05</v>
       </c>
-      <c r="H42" t="n">
+      <c r="I42" t="n">
         <v>0.0002991914749145508</v>
       </c>
-      <c r="I42" t="n">
-        <v>100</v>
-      </c>
       <c r="J42" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="K42" t="n">
+        <v>0</v>
+      </c>
+      <c r="L42" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1775,32 +1903,35 @@
       <c r="A43" s="1" t="n">
         <v>41</v>
       </c>
-      <c r="B43" t="inlineStr">
+      <c r="B43" t="n">
+        <v>6</v>
+      </c>
+      <c r="C43" t="inlineStr">
         <is>
           <t>usa_csp</t>
         </is>
       </c>
-      <c r="C43" t="n">
+      <c r="D43" t="n">
         <v>65.40000000000001</v>
       </c>
-      <c r="D43" t="n">
+      <c r="E43" t="n">
         <v>33.8325287260648</v>
       </c>
-      <c r="E43" t="inlineStr"/>
       <c r="F43" t="inlineStr"/>
-      <c r="G43" t="n">
+      <c r="G43" t="inlineStr"/>
+      <c r="H43" t="n">
         <v>0.00409245491027832</v>
       </c>
-      <c r="H43" t="n">
+      <c r="I43" t="n">
         <v>0.007867821431155574</v>
       </c>
-      <c r="I43" t="n">
-        <v>100</v>
-      </c>
       <c r="J43" t="n">
+        <v>100</v>
+      </c>
+      <c r="K43" t="n">
         <v>16.4</v>
       </c>
-      <c r="K43" t="n">
+      <c r="L43" t="n">
         <v>33.83252872606479</v>
       </c>
     </row>
@@ -1808,32 +1939,35 @@
       <c r="A44" s="1" t="n">
         <v>42</v>
       </c>
-      <c r="B44" t="inlineStr">
+      <c r="B44" t="n">
+        <v>6</v>
+      </c>
+      <c r="C44" t="inlineStr">
         <is>
           <t>zebra</t>
         </is>
       </c>
-      <c r="C44" t="n">
+      <c r="D44" t="n">
         <v>996.7</v>
       </c>
-      <c r="D44" t="n">
+      <c r="E44" t="n">
         <v>84.90000000000001</v>
       </c>
-      <c r="E44" t="inlineStr"/>
       <c r="F44" t="inlineStr"/>
-      <c r="G44" t="n">
+      <c r="G44" t="inlineStr"/>
+      <c r="H44" t="n">
         <v>0.2547230243682861</v>
       </c>
-      <c r="H44" t="n">
+      <c r="I44" t="n">
         <v>0.023088942403766</v>
       </c>
-      <c r="I44" t="n">
+      <c r="J44" t="n">
         <v>10</v>
       </c>
-      <c r="J44" t="n">
+      <c r="K44" t="n">
         <v>971.7</v>
       </c>
-      <c r="K44" t="n">
+      <c r="L44" t="n">
         <v>84.90000000000001</v>
       </c>
     </row>
@@ -1841,32 +1975,35 @@
       <c r="A45" s="1" t="n">
         <v>43</v>
       </c>
-      <c r="B45" t="inlineStr">
+      <c r="B45" t="n">
+        <v>6</v>
+      </c>
+      <c r="C45" t="inlineStr">
         <is>
           <t>10 queens</t>
         </is>
       </c>
-      <c r="C45" t="n">
+      <c r="D45" t="n">
         <v>93.7</v>
       </c>
-      <c r="D45" t="n">
+      <c r="E45" t="n">
         <v>73.87969951211225</v>
       </c>
-      <c r="E45" t="inlineStr"/>
       <c r="F45" t="inlineStr"/>
-      <c r="G45" t="n">
+      <c r="G45" t="inlineStr"/>
+      <c r="H45" t="n">
         <v>0.002894377708435059</v>
       </c>
-      <c r="H45" t="n">
+      <c r="I45" t="n">
         <v>0.002704243078069995</v>
       </c>
-      <c r="I45" t="n">
-        <v>100</v>
-      </c>
       <c r="J45" t="n">
+        <v>100</v>
+      </c>
+      <c r="K45" t="n">
         <v>83.7</v>
       </c>
-      <c r="K45" t="n">
+      <c r="L45" t="n">
         <v>73.87969951211225</v>
       </c>
     </row>
@@ -1874,32 +2011,35 @@
       <c r="A46" s="1" t="n">
         <v>44</v>
       </c>
-      <c r="B46" t="inlineStr">
+      <c r="B46" t="n">
+        <v>6</v>
+      </c>
+      <c r="C46" t="inlineStr">
         <is>
           <t>30 queens</t>
         </is>
       </c>
-      <c r="C46" t="n">
+      <c r="D46" t="n">
         <v>65.7</v>
       </c>
-      <c r="D46" t="n">
+      <c r="E46" t="n">
         <v>13.37198564163154</v>
       </c>
-      <c r="E46" t="inlineStr"/>
       <c r="F46" t="inlineStr"/>
-      <c r="G46" t="n">
+      <c r="G46" t="inlineStr"/>
+      <c r="H46" t="n">
         <v>0.003189349174499512</v>
       </c>
-      <c r="H46" t="n">
+      <c r="I46" t="n">
         <v>0.0008733219534624252</v>
       </c>
-      <c r="I46" t="n">
-        <v>100</v>
-      </c>
       <c r="J46" t="n">
+        <v>100</v>
+      </c>
+      <c r="K46" t="n">
         <v>35.7</v>
       </c>
-      <c r="K46" t="n">
+      <c r="L46" t="n">
         <v>13.37198564163154</v>
       </c>
     </row>
@@ -1907,32 +2047,35 @@
       <c r="A47" s="1" t="n">
         <v>45</v>
       </c>
-      <c r="B47" t="inlineStr">
+      <c r="B47" t="n">
+        <v>6</v>
+      </c>
+      <c r="C47" t="inlineStr">
         <is>
           <t>50 queens</t>
         </is>
       </c>
-      <c r="C47" t="n">
+      <c r="D47" t="n">
         <v>102.1</v>
       </c>
-      <c r="D47" t="n">
+      <c r="E47" t="n">
         <v>29.63595788902393</v>
       </c>
-      <c r="E47" t="inlineStr"/>
       <c r="F47" t="inlineStr"/>
-      <c r="G47" t="n">
+      <c r="G47" t="inlineStr"/>
+      <c r="H47" t="n">
         <v>0.00718083381652832</v>
       </c>
-      <c r="H47" t="n">
+      <c r="I47" t="n">
         <v>0.003082503587928742</v>
       </c>
-      <c r="I47" t="n">
-        <v>100</v>
-      </c>
       <c r="J47" t="n">
+        <v>100</v>
+      </c>
+      <c r="K47" t="n">
         <v>52.1</v>
       </c>
-      <c r="K47" t="n">
+      <c r="L47" t="n">
         <v>29.63595788902393</v>
       </c>
     </row>
@@ -1940,32 +2083,35 @@
       <c r="A48" s="1" t="n">
         <v>46</v>
       </c>
-      <c r="B48" t="inlineStr">
+      <c r="B48" t="n">
+        <v>6</v>
+      </c>
+      <c r="C48" t="inlineStr">
         <is>
           <t>70 queens</t>
         </is>
       </c>
-      <c r="C48" t="n">
+      <c r="D48" t="n">
         <v>132.4</v>
       </c>
-      <c r="D48" t="n">
+      <c r="E48" t="n">
         <v>19.7038067388005</v>
       </c>
-      <c r="E48" t="inlineStr"/>
       <c r="F48" t="inlineStr"/>
-      <c r="G48" t="n">
+      <c r="G48" t="inlineStr"/>
+      <c r="H48" t="n">
         <v>0.01237592697143555</v>
       </c>
-      <c r="H48" t="n">
+      <c r="I48" t="n">
         <v>0.002247189484898627</v>
       </c>
-      <c r="I48" t="n">
-        <v>100</v>
-      </c>
       <c r="J48" t="n">
+        <v>100</v>
+      </c>
+      <c r="K48" t="n">
         <v>62.4</v>
       </c>
-      <c r="K48" t="n">
+      <c r="L48" t="n">
         <v>19.7038067388005</v>
       </c>
     </row>
@@ -1973,32 +2119,35 @@
       <c r="A49" s="1" t="n">
         <v>47</v>
       </c>
-      <c r="B49" t="inlineStr">
+      <c r="B49" t="n">
+        <v>6</v>
+      </c>
+      <c r="C49" t="inlineStr">
         <is>
           <t>90 queens</t>
         </is>
       </c>
-      <c r="C49" t="n">
+      <c r="D49" t="n">
         <v>137.4</v>
       </c>
-      <c r="D49" t="n">
+      <c r="E49" t="n">
         <v>50.32335441919587</v>
       </c>
-      <c r="E49" t="inlineStr"/>
       <c r="F49" t="inlineStr"/>
-      <c r="G49" t="n">
+      <c r="G49" t="inlineStr"/>
+      <c r="H49" t="n">
         <v>0.01565613746643067</v>
       </c>
-      <c r="H49" t="n">
+      <c r="I49" t="n">
         <v>0.007151623250998417</v>
       </c>
-      <c r="I49" t="n">
-        <v>100</v>
-      </c>
       <c r="J49" t="n">
+        <v>100</v>
+      </c>
+      <c r="K49" t="n">
         <v>47.4</v>
       </c>
-      <c r="K49" t="n">
+      <c r="L49" t="n">
         <v>50.32335441919587</v>
       </c>
     </row>

</xml_diff>